<commit_message>
ahora en principio guardara todos los datos en el mismo excel, para tener un registro completo
</commit_message>
<xml_diff>
--- a/Tarragona_weather_data.xlsx
+++ b/Tarragona_weather_data.xlsx
@@ -1,34 +1,106 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Programacion\python\Weather\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EA25DB-E6BD-4A3D-8DAB-14F97011F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+  <si>
+    <t>coord</t>
+  </si>
+  <si>
+    <t>{'lon': 1.249, 'lat': 41.129}</t>
+  </si>
+  <si>
+    <t>weather</t>
+  </si>
+  <si>
+    <t>[{'id': 800, 'main': 'Clear', 'description': 'clear sky', 'icon': '01d'}]</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>stations</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>{'temp': 287.38, 'feels_like': 286.43, 'temp_min': 286.06, 'temp_max': 289.68, 'pressure': 1021, 'humidity': 60}</t>
+  </si>
+  <si>
+    <t>visibility</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>{'speed': 3.13, 'deg': 245, 'gust': 4.47}</t>
+  </si>
+  <si>
+    <t>clouds</t>
+  </si>
+  <si>
+    <t>{'all': 0}</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>sys</t>
+  </si>
+  <si>
+    <t>{'type': 2, 'id': 2010267, 'country': 'ES', 'sunrise': 1703834380, 'sunset': 1703867624}</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Tarragona</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +119,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,162 +421,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>coord</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>{'lon': 1.249, 'lat': 41.129}</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>weather</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[{'id': 800, 'main': 'Clear', 'description': 'clear sky', 'icon': '01d'}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>stations</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>main</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>{'temp': 287.38, 'feels_like': 286.43, 'temp_min': 286.06, 'temp_max': 289.68, 'pressure': 1021, 'humidity': 60}</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>visibility</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>10000</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>wind</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>{'speed': 3.13, 'deg': 245, 'gust': 4.47}</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>clouds</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>{'all': 0}</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>dt</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
         <v>1703850638</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sys</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>{'type': 2, 'id': 2010267, 'country': 'ES', 'sunrise': 1703834380, 'sunset': 1703867624}</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>timezone</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
         <v>3600</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
         <v>3108287</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Tarragona</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cod</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>1703850638</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>3108287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ahora si que pone los datos en la primera celda vacia que encuentre
</commit_message>
<xml_diff>
--- a/Tarragona_weather_data.xlsx
+++ b/Tarragona_weather_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Programacion\python\Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EA25DB-E6BD-4A3D-8DAB-14F97011F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B0848F-DCFE-400F-9ABD-0682F93A394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>coord</t>
   </si>
@@ -31,7 +31,7 @@
     <t>weather</t>
   </si>
   <si>
-    <t>[{'id': 800, 'main': 'Clear', 'description': 'clear sky', 'icon': '01d'}]</t>
+    <t>[{'id': 800, 'main': 'Clear', 'description': 'clear sky', 'icon': '01n'}]</t>
   </si>
   <si>
     <t>base</t>
@@ -43,7 +43,7 @@
     <t>main</t>
   </si>
   <si>
-    <t>{'temp': 287.38, 'feels_like': 286.43, 'temp_min': 286.06, 'temp_max': 289.68, 'pressure': 1021, 'humidity': 60}</t>
+    <t>{'temp': 285.5, 'feels_like': 284.8, 'temp_min': 283.92, 'temp_max': 285.96, 'pressure': 1018, 'humidity': 77}</t>
   </si>
   <si>
     <t>visibility</t>
@@ -52,7 +52,7 @@
     <t>wind</t>
   </si>
   <si>
-    <t>{'speed': 3.13, 'deg': 245, 'gust': 4.47}</t>
+    <t>{'speed': 1.54, 'deg': 190}</t>
   </si>
   <si>
     <t>clouds</t>
@@ -67,7 +67,7 @@
     <t>sys</t>
   </si>
   <si>
-    <t>{'type': 2, 'id': 2010267, 'country': 'ES', 'sunrise': 1703834380, 'sunset': 1703867624}</t>
+    <t>{'type': 2, 'id': 2010267, 'country': 'ES', 'sunrise': 1703920793, 'sunset': 1703954067}</t>
   </si>
   <si>
     <t>timezone</t>
@@ -89,13 +89,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,7 +112,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -116,10 +129,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,6 +231,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -246,6 +266,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -269,7 +290,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -280,31 +300,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -326,7 +346,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -384,7 +404,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -397,13 +417,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -422,15 +441,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:L119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -446,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -454,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -462,15 +488,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -478,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -486,15 +512,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>1703850638</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1703954724</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -502,23 +528,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>3600</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>3108287</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -526,119 +552,169 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21">
-        <v>1703850638</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24">
-        <v>3108287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26">
-        <v>200</v>
-      </c>
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pone los datos ordenados en excel pero no los separa del todo bien
</commit_message>
<xml_diff>
--- a/Tarragona_weather_data.xlsx
+++ b/Tarragona_weather_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Programacion\python\Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B0848F-DCFE-400F-9ABD-0682F93A394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6512C8DD-C590-4D1E-98EA-46922C40DF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
   <si>
     <t>coord</t>
   </si>
@@ -89,19 +95,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,14 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -129,16 +122,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,7 +218,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -266,7 +252,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,6 +275,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -300,31 +286,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -346,7 +332,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -404,7 +390,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -417,12 +403,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -441,22 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:L119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -472,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -480,7 +460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -488,23 +468,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -512,209 +492,63 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>1703954724</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1703955336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
         <v>3600</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
         <v>3108287</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>